<commit_message>
previous and refresh page
</commit_message>
<xml_diff>
--- a/veg_data/basic_vege_202507211504_good.xlsx
+++ b/veg_data/basic_vege_202507211504_good.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\veg_read\veg_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\veg_linebot\veg_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BF7C969-CA50-4E56-A205-8D81DAC00290}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68396B0B-93F9-4BC8-B38F-6D601A07C5A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,9 +376,6 @@
     <t>SF1</t>
   </si>
   <si>
-    <t>蒜</t>
-  </si>
-  <si>
     <t>SG5</t>
   </si>
   <si>
@@ -389,6 +386,10 @@
   </si>
   <si>
     <t>vege_id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒜頭</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -399,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -431,6 +432,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -452,12 +460,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -678,8 +687,8 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,7 +698,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1345,15 +1354,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>35</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,10 +1370,10 @@
         <v>25</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>